<commit_message>
reporte anual y mensual funcionando correctamente
</commit_message>
<xml_diff>
--- a/public/application/files/jasper/templates/flujoefectivomensual1B.xlsx
+++ b/public/application/files/jasper/templates/flujoefectivomensual1B.xlsx
@@ -223,17 +223,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -247,22 +238,32 @@
       <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="10" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="7" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="2" fontId="6" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="2" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -599,7 +600,7 @@
   <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -608,110 +609,110 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="29.75" customHeight="1">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
     </row>
     <row r="2" spans="1:4" ht="29.75" customHeight="1">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
+      <c r="B2" s="13"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
     </row>
     <row r="3" spans="1:4" ht="28">
-      <c r="A3" s="3"/>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
+      <c r="A3" s="13"/>
+      <c r="B3" s="13"/>
+      <c r="C3" s="13"/>
+      <c r="D3" s="13"/>
     </row>
     <row r="4" spans="1:4" ht="22.25" customHeight="1">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
+      <c r="B4" s="14"/>
+      <c r="C4" s="14"/>
+      <c r="D4" s="14"/>
     </row>
     <row r="5" spans="1:4" ht="18">
-      <c r="A5" s="17" t="s">
+      <c r="A5" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="17" t="s">
+      <c r="C5" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D5" s="1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:4">
-      <c r="A6" s="1"/>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-    </row>
-    <row r="7" spans="1:4" s="8" customFormat="1">
-      <c r="A7" s="5" t="s">
+      <c r="A6" s="12"/>
+      <c r="B6" s="12"/>
+      <c r="C6" s="12"/>
+      <c r="D6" s="12"/>
+    </row>
+    <row r="7" spans="1:4" s="5" customFormat="1">
+      <c r="A7" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="C7" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D7" s="7" t="s">
+      <c r="D7" s="4" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:4">
-      <c r="A8" s="9" t="s">
+      <c r="A8" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="10" t="s">
+      <c r="B8" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="18" t="s">
+      <c r="C8" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="D8" s="19" t="s">
+      <c r="D8" s="20" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:4">
-      <c r="A9" s="11"/>
-      <c r="B9" s="12"/>
-      <c r="C9" s="12"/>
-      <c r="D9" s="12"/>
+      <c r="A9" s="7"/>
+      <c r="B9" s="8"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="8"/>
     </row>
     <row r="14" spans="1:4">
-      <c r="A14" s="13" t="s">
+      <c r="A14" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="B14" s="13" t="s">
+      <c r="B14" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="C14" s="13" t="s">
+      <c r="C14" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="D14" s="13" t="s">
+      <c r="D14" s="17" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="16" spans="1:4">
-      <c r="A16" s="14" t="s">
+      <c r="A16" s="10" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="17" spans="1:4">
-      <c r="A17" s="13" t="s">
+      <c r="A17" s="9" t="s">
         <v>15</v>
       </c>
       <c r="B17" s="15" t="s">
@@ -734,7 +735,6 @@
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0249999999999999" bottom="1.0249999999999999" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>

</xml_diff>